<commit_message>
added auth and leads apis
</commit_message>
<xml_diff>
--- a/Crackteck-modules.xlsx
+++ b/Crackteck-modules.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECHNOFRA-SACHIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crackteck-git\crackteck-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1305,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1714,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>13</v>
       </c>
@@ -1798,8 +1798,8 @@
       <c r="D35" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="68" t="s">
-        <v>129</v>
+      <c r="E35" s="65" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1815,8 +1815,8 @@
       <c r="D36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="67" t="s">
-        <v>132</v>
+      <c r="E36" s="65" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2089,8 +2089,8 @@
       <c r="D59" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="68" t="s">
-        <v>130</v>
+      <c r="E59" s="67" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2185,8 +2185,8 @@
       <c r="D65" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E65" s="67" t="s">
-        <v>132</v>
+      <c r="E65" s="65" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2202,8 +2202,8 @@
       <c r="D66" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E66" s="68" t="s">
-        <v>130</v>
+      <c r="E66" s="65" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2389,7 +2389,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="57" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D80" s="63" t="s">
         <v>28</v>

</xml_diff>